<commit_message>
update staff info page
</commit_message>
<xml_diff>
--- a/RapidTest/wwwroot/excelTemplate/employee.xlsx
+++ b/RapidTest/wwwroot/excelTemplate/employee.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\a_todolist\2021\RapidTest\RapidTest\wwwroot\excelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A00E29-89AC-416C-BCEF-5578B142A4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BCB601-C1B8-4BA1-8DB8-161BD427B5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="972" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Factory</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>NĂM SINH(mm/dd/yyyy)</t>
+  </si>
+  <si>
+    <t>Print: ON/OFF</t>
+  </si>
+  <si>
+    <t>OFF</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,9 +460,10 @@
     <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +485,11 @@
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -501,8 +511,11 @@
       <c r="G2" s="4" t="b">
         <v>1</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -524,8 +537,11 @@
       <c r="G3" s="4" t="b">
         <v>1</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -546,6 +562,9 @@
       </c>
       <c r="G4" s="4" t="b">
         <v>1</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update new demand staff info
</commit_message>
<xml_diff>
--- a/RapidTest/wwwroot/excelTemplate/employee.xlsx
+++ b/RapidTest/wwwroot/excelTemplate/employee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\a_todolist\2021\RapidTest\RapidTest\wwwroot\excelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AA64AC-CC4D-4EAF-A002-F642DB0C515A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B0DD4E-C196-481B-861F-7AAD95A20463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1032" yWindow="1356" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>SHC</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -191,6 +191,53 @@
   </si>
   <si>
     <t>Ghi chú: Những cột chứa dấu (*) là bắt buộc nhập.</t>
+  </si>
+  <si>
+    <t>1 = Sunday</t>
+  </si>
+  <si>
+    <t>2 = Monday</t>
+  </si>
+  <si>
+    <t>3 = Tuesday</t>
+  </si>
+  <si>
+    <t>4 = Wednesday</t>
+  </si>
+  <si>
+    <t>5 = Thursday</t>
+  </si>
+  <si>
+    <t>6 = Friday</t>
+  </si>
+  <si>
+    <t>7 = Saturday</t>
+  </si>
+  <si>
+    <t>Để trống là tất cả các ngày trong tuần</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ngày Xét Nghiệm </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <t>Dữ Liệu Ngày Xét Nghiệm (Test Date)</t>
+  </si>
+  <si>
+    <t>2.4.6</t>
+  </si>
+  <si>
+    <t>3.5.7</t>
   </si>
 </sst>
 </file>
@@ -200,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +287,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -255,7 +307,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -263,11 +315,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -286,11 +353,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,10 +659,12 @@
     <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.109375" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="10" max="10" width="29.77734375" style="8" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.77734375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="39.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -620,12 +692,17 @@
       <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -653,8 +730,14 @@
       <c r="I2" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -682,8 +765,14 @@
       <c r="I3" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -710,11 +799,39 @@
       </c>
       <c r="I4" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L5" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L6" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L7" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L8" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L9" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J1:J1048576"/>
+    <mergeCell ref="K1:K1048576"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>